<commit_message>
Maximum gewicht load toegevoegd
</commit_message>
<xml_diff>
--- a/Documentation/Requirements and Wishes.xlsx
+++ b/Documentation/Requirements and Wishes.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="17766"/>
-  <workbookPr defaultThemeVersion="166925"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="17329"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\radel\Documents\GitHub\MinorAR_MultiRobot\Documentation\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Remco\Documents\MinorAR_MultiRobot\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7530"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20496" windowHeight="7536"/>
   </bookViews>
   <sheets>
     <sheet name="Blad1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="27">
   <si>
     <t>Requirements</t>
   </si>
@@ -102,6 +102,9 @@
   </si>
   <si>
     <t>The Turtlebot's max payload is 5kg</t>
+  </si>
+  <si>
+    <t>The maximum load to be moved will be +/- 2 kg</t>
   </si>
 </sst>
 </file>
@@ -462,144 +465,149 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:B28"/>
+  <dimension ref="B2:B30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B22" sqref="B22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="70.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="70.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B2" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B3" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B4" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B5" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B6" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B7" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B8" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="9" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B9" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="10" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B10" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="11" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B11" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="12" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B12" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="13" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B13" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="14" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B14" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="15" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B15" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="16" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B16" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="17" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B17" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="18" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B18" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="19" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B19" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="20" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B20" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="22" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B22" s="1" t="s">
+    <row r="21" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B21" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="24" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B24" s="1" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="23" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B23" t="s">
+    <row r="25" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B25" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="24" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B24" t="s">
+    <row r="26" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B26" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="25" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B25" t="s">
+    <row r="27" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B27" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="26" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B26" t="s">
+    <row r="28" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B28" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="27" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B27" t="s">
+    <row r="29" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B29" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="28" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B28" t="s">
+    <row r="30" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B30" t="s">
         <v>24</v>
       </c>
     </row>

</xml_diff>